<commit_message>
chore: update sample reports
</commit_message>
<xml_diff>
--- a/services/worker/scripts/report/output/expenses/last_month/expenses-last_month.xlsx
+++ b/services/worker/scripts/report/output/expenses/last_month/expenses-last_month.xlsx
@@ -5,226 +5,241 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="סיכום" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="חשבוניות" state="visible" r:id="rId5"/>
+    <sheet sheetId="2" name="הוצאות" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>דוח הוצאות - דוגמה בע"מ - Demo Business Ltd</t>
   </si>
   <si>
-    <t>תקופה: 2025-12-01 עד 2025-12-31</t>
-  </si>
-  <si>
-    <t>סה"כ הוצאות (לפי מטבע)</t>
+    <t>תקופה: 2026-01-01 עד 2026-01-31</t>
+  </si>
+  <si>
+    <t>סה"כ לפי מטבע</t>
+  </si>
+  <si>
+    <t>ILS - סה"כ</t>
+  </si>
+  <si>
+    <t>₪22,950</t>
+  </si>
+  <si>
+    <t>USD - סה"כ</t>
+  </si>
+  <si>
+    <t>$2,800</t>
+  </si>
+  <si>
+    <t>EUR - סה"כ</t>
+  </si>
+  <si>
+    <t>€850</t>
+  </si>
+  <si>
+    <t>מדד</t>
+  </si>
+  <si>
+    <t>ערך</t>
+  </si>
+  <si>
+    <t>סה"כ הוצאות (ILS)</t>
+  </si>
+  <si>
+    <t>₪26,600</t>
+  </si>
+  <si>
+    <t>מספר הוצאות</t>
+  </si>
+  <si>
+    <t>ממוצע לחשבונית (ILS)</t>
+  </si>
+  <si>
+    <t>₪1773.33</t>
+  </si>
+  <si>
+    <t>חשבונית מקסימלית (ILS)</t>
+  </si>
+  <si>
+    <t>₪4,500</t>
+  </si>
+  <si>
+    <t>חשבונית מינימלית (ILS)</t>
+  </si>
+  <si>
+    <t>₪250</t>
+  </si>
+  <si>
+    <t>תאריך</t>
+  </si>
+  <si>
+    <t>ספק</t>
+  </si>
+  <si>
+    <t>סכום</t>
+  </si>
+  <si>
+    <t>מטבע</t>
+  </si>
+  <si>
+    <t>אמצעי תשלום</t>
+  </si>
+  <si>
+    <t>קטגוריה</t>
+  </si>
+  <si>
+    <t>קישור</t>
+  </si>
+  <si>
+    <t>2026-01-01</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform</t>
   </si>
   <si>
     <t>ILS</t>
   </si>
   <si>
-    <t>₪22,950</t>
+    <t>כרטיס אשראי</t>
+  </si>
+  <si>
+    <t>שירותי ענן</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-001.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-03</t>
+  </si>
+  <si>
+    <t>משרד רואה חשבון</t>
+  </si>
+  <si>
+    <t>העברה בנקאית</t>
+  </si>
+  <si>
+    <t>שירותים מקצועיים</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-002.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-05</t>
+  </si>
+  <si>
+    <t>Office Depot</t>
+  </si>
+  <si>
+    <t>ציוד משרדי</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-003.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-07</t>
+  </si>
+  <si>
+    <t>חברת חשמל</t>
+  </si>
+  <si>
+    <t>חשבונות</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-004.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-09</t>
+  </si>
+  <si>
+    <t>GitHub Enterprise</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>$2,800</t>
+    <t>תוכנה</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-005.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-11</t>
+  </si>
+  <si>
+    <t>משרד עורך דין</t>
+  </si>
+  <si>
+    <t>שירותים משפטיים</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-006.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-13</t>
+  </si>
+  <si>
+    <t>LinkedIn Premium</t>
+  </si>
+  <si>
+    <t>שיווק</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-007.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-15</t>
+  </si>
+  <si>
+    <t>בזק בינלאומי</t>
+  </si>
+  <si>
+    <t>תקשורת</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-008.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-17</t>
+  </si>
+  <si>
+    <t>Adobe Creative Cloud</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-009.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-19</t>
+  </si>
+  <si>
+    <t>משלוח ארוחות</t>
+  </si>
+  <si>
+    <t>מזומן</t>
+  </si>
+  <si>
+    <t>אירוח</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-010.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-21</t>
+  </si>
+  <si>
+    <t>AWS</t>
   </si>
   <si>
     <t>EUR</t>
   </si>
   <si>
-    <t>€850</t>
-  </si>
-  <si>
-    <t>מדד</t>
-  </si>
-  <si>
-    <t>ערך</t>
-  </si>
-  <si>
-    <t>מספר חשבוניות (ILS)</t>
-  </si>
-  <si>
-    <t>ממוצע לחשבונית (ILS)</t>
-  </si>
-  <si>
-    <t>₪1912.50</t>
-  </si>
-  <si>
-    <t>חשבונית מקסימלית (ILS)</t>
-  </si>
-  <si>
-    <t>₪4,500</t>
-  </si>
-  <si>
-    <t>חשבונית מינימלית (ILS)</t>
-  </si>
-  <si>
-    <t>₪250</t>
-  </si>
-  <si>
-    <t>תאריך</t>
-  </si>
-  <si>
-    <t>לקוח</t>
-  </si>
-  <si>
-    <t>סכום</t>
-  </si>
-  <si>
-    <t>מטבע</t>
-  </si>
-  <si>
-    <t>אמצעי תשלום</t>
-  </si>
-  <si>
-    <t>קטגוריה</t>
-  </si>
-  <si>
-    <t>קישור</t>
-  </si>
-  <si>
-    <t>2025-12-01</t>
-  </si>
-  <si>
-    <t>Google Cloud Platform</t>
-  </si>
-  <si>
-    <t>כרטיס אשראי</t>
-  </si>
-  <si>
-    <t>שירותי ענן</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-001.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-03</t>
-  </si>
-  <si>
-    <t>משרד רואה חשבון</t>
-  </si>
-  <si>
-    <t>העברה בנקאית</t>
-  </si>
-  <si>
-    <t>שירותים מקצועיים</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-002.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-05</t>
-  </si>
-  <si>
-    <t>Office Depot</t>
-  </si>
-  <si>
-    <t>ציוד משרדי</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-003.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-07</t>
-  </si>
-  <si>
-    <t>חברת חשמל</t>
-  </si>
-  <si>
-    <t>חשבונות</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-004.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-09</t>
-  </si>
-  <si>
-    <t>GitHub Enterprise</t>
-  </si>
-  <si>
-    <t>תוכנה</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-005.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-11</t>
-  </si>
-  <si>
-    <t>משרד עורך דין</t>
-  </si>
-  <si>
-    <t>שירותים משפטיים</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-006.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-13</t>
-  </si>
-  <si>
-    <t>LinkedIn Premium</t>
-  </si>
-  <si>
-    <t>שיווק</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-007.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-15</t>
-  </si>
-  <si>
-    <t>בזק בינלאומי</t>
-  </si>
-  <si>
-    <t>תקשורת</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-008.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-17</t>
-  </si>
-  <si>
-    <t>Adobe Creative Cloud</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-009.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-19</t>
-  </si>
-  <si>
-    <t>משלוח ארוחות</t>
-  </si>
-  <si>
-    <t>מזומן</t>
-  </si>
-  <si>
-    <t>אירוח</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-010.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-21</t>
-  </si>
-  <si>
-    <t>AWS</t>
-  </si>
-  <si>
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-011.pdf</t>
   </si>
   <si>
-    <t>2025-12-23</t>
+    <t>2026-01-23</t>
   </si>
   <si>
     <t>חניון חודשי</t>
@@ -236,7 +251,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-012.pdf</t>
   </si>
   <si>
-    <t>2025-12-25</t>
+    <t>2026-01-25</t>
   </si>
   <si>
     <t>Zoom Pro</t>
@@ -245,7 +260,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-013.pdf</t>
   </si>
   <si>
-    <t>2025-12-27</t>
+    <t>2026-01-27</t>
   </si>
   <si>
     <t>ביטוח לאומי</t>
@@ -257,7 +272,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-014.pdf</t>
   </si>
   <si>
-    <t>2025-12-29</t>
+    <t>2026-01-29</t>
   </si>
   <si>
     <t>ניקיון משרדים</t>
@@ -677,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="1"/>
   </sheetViews>
@@ -744,32 +759,40 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B11">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -801,370 +824,370 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5">
         <v>4500</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5">
         <v>3200</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5">
         <v>850</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5">
         <v>650</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5">
         <v>1800</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5">
         <v>4200</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5">
         <v>350</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5">
         <v>450</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C10" s="5">
         <v>1000</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5">
         <v>950</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C12" s="5">
         <v>850</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C13" s="5">
         <v>700</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C14" s="5">
         <v>550</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C15" s="5">
         <v>3600</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C16" s="5">
         <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat/payment tracking in reports (#145)
* refactor: consolidate InvoiceDocumentType and remove unused counter function

  - Consolidate inline 'invoice' | 'receipt' | 'invoice_receipt' types to single InvoiceDocumentType
  - Remove unused getCurrentCounter() function from counter.service

* feat: add payment status tracking to report types

* feat: implement payment tracking and collection rate in reports

  - Update report service to map payment status fields from invoices
  - Rewrite calculateMetrics to distinguish invoiced vs received amounts
  - Add payment status badges (שולם/ממתין/חלקי) to PDF reports
  - Add collection rate display (אחוז גביה) to summary section
  - Format all amounts with toLocaleString() for comma separators
  - Filter linked receipts to prevent double-counting in metrics

* chore: update sample reports

* test: update tests

* chore: update readme

* test: fix

* test: add uts
</commit_message>
<xml_diff>
--- a/services/worker/scripts/report/output/expenses/last_month/expenses-last_month.xlsx
+++ b/services/worker/scripts/report/output/expenses/last_month/expenses-last_month.xlsx
@@ -5,226 +5,241 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="סיכום" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="חשבוניות" state="visible" r:id="rId5"/>
+    <sheet sheetId="2" name="הוצאות" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>דוח הוצאות - דוגמה בע"מ - Demo Business Ltd</t>
   </si>
   <si>
-    <t>תקופה: 2025-12-01 עד 2025-12-31</t>
-  </si>
-  <si>
-    <t>סה"כ הוצאות (לפי מטבע)</t>
+    <t>תקופה: 2026-01-01 עד 2026-01-31</t>
+  </si>
+  <si>
+    <t>סה"כ לפי מטבע</t>
+  </si>
+  <si>
+    <t>ILS - סה"כ</t>
+  </si>
+  <si>
+    <t>₪22,950</t>
+  </si>
+  <si>
+    <t>USD - סה"כ</t>
+  </si>
+  <si>
+    <t>$2,800</t>
+  </si>
+  <si>
+    <t>EUR - סה"כ</t>
+  </si>
+  <si>
+    <t>€850</t>
+  </si>
+  <si>
+    <t>מדד</t>
+  </si>
+  <si>
+    <t>ערך</t>
+  </si>
+  <si>
+    <t>סה"כ הוצאות (ILS)</t>
+  </si>
+  <si>
+    <t>₪26,600</t>
+  </si>
+  <si>
+    <t>מספר הוצאות</t>
+  </si>
+  <si>
+    <t>ממוצע לחשבונית (ILS)</t>
+  </si>
+  <si>
+    <t>₪1773.33</t>
+  </si>
+  <si>
+    <t>חשבונית מקסימלית (ILS)</t>
+  </si>
+  <si>
+    <t>₪4,500</t>
+  </si>
+  <si>
+    <t>חשבונית מינימלית (ILS)</t>
+  </si>
+  <si>
+    <t>₪250</t>
+  </si>
+  <si>
+    <t>תאריך</t>
+  </si>
+  <si>
+    <t>ספק</t>
+  </si>
+  <si>
+    <t>סכום</t>
+  </si>
+  <si>
+    <t>מטבע</t>
+  </si>
+  <si>
+    <t>אמצעי תשלום</t>
+  </si>
+  <si>
+    <t>קטגוריה</t>
+  </si>
+  <si>
+    <t>קישור</t>
+  </si>
+  <si>
+    <t>2026-01-01</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform</t>
   </si>
   <si>
     <t>ILS</t>
   </si>
   <si>
-    <t>₪22,950</t>
+    <t>כרטיס אשראי</t>
+  </si>
+  <si>
+    <t>שירותי ענן</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-001.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-03</t>
+  </si>
+  <si>
+    <t>משרד רואה חשבון</t>
+  </si>
+  <si>
+    <t>העברה בנקאית</t>
+  </si>
+  <si>
+    <t>שירותים מקצועיים</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-002.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-05</t>
+  </si>
+  <si>
+    <t>Office Depot</t>
+  </si>
+  <si>
+    <t>ציוד משרדי</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-003.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-07</t>
+  </si>
+  <si>
+    <t>חברת חשמל</t>
+  </si>
+  <si>
+    <t>חשבונות</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-004.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-09</t>
+  </si>
+  <si>
+    <t>GitHub Enterprise</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>$2,800</t>
+    <t>תוכנה</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-005.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-11</t>
+  </si>
+  <si>
+    <t>משרד עורך דין</t>
+  </si>
+  <si>
+    <t>שירותים משפטיים</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-006.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-13</t>
+  </si>
+  <si>
+    <t>LinkedIn Premium</t>
+  </si>
+  <si>
+    <t>שיווק</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-007.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-15</t>
+  </si>
+  <si>
+    <t>בזק בינלאומי</t>
+  </si>
+  <si>
+    <t>תקשורת</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-008.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-17</t>
+  </si>
+  <si>
+    <t>Adobe Creative Cloud</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-009.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-19</t>
+  </si>
+  <si>
+    <t>משלוח ארוחות</t>
+  </si>
+  <si>
+    <t>מזומן</t>
+  </si>
+  <si>
+    <t>אירוח</t>
+  </si>
+  <si>
+    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-010.pdf</t>
+  </si>
+  <si>
+    <t>2026-01-21</t>
+  </si>
+  <si>
+    <t>AWS</t>
   </si>
   <si>
     <t>EUR</t>
   </si>
   <si>
-    <t>€850</t>
-  </si>
-  <si>
-    <t>מדד</t>
-  </si>
-  <si>
-    <t>ערך</t>
-  </si>
-  <si>
-    <t>מספר חשבוניות (ILS)</t>
-  </si>
-  <si>
-    <t>ממוצע לחשבונית (ILS)</t>
-  </si>
-  <si>
-    <t>₪1912.50</t>
-  </si>
-  <si>
-    <t>חשבונית מקסימלית (ILS)</t>
-  </si>
-  <si>
-    <t>₪4,500</t>
-  </si>
-  <si>
-    <t>חשבונית מינימלית (ILS)</t>
-  </si>
-  <si>
-    <t>₪250</t>
-  </si>
-  <si>
-    <t>תאריך</t>
-  </si>
-  <si>
-    <t>לקוח</t>
-  </si>
-  <si>
-    <t>סכום</t>
-  </si>
-  <si>
-    <t>מטבע</t>
-  </si>
-  <si>
-    <t>אמצעי תשלום</t>
-  </si>
-  <si>
-    <t>קטגוריה</t>
-  </si>
-  <si>
-    <t>קישור</t>
-  </si>
-  <si>
-    <t>2025-12-01</t>
-  </si>
-  <si>
-    <t>Google Cloud Platform</t>
-  </si>
-  <si>
-    <t>כרטיס אשראי</t>
-  </si>
-  <si>
-    <t>שירותי ענן</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-001.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-03</t>
-  </si>
-  <si>
-    <t>משרד רואה חשבון</t>
-  </si>
-  <si>
-    <t>העברה בנקאית</t>
-  </si>
-  <si>
-    <t>שירותים מקצועיים</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-002.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-05</t>
-  </si>
-  <si>
-    <t>Office Depot</t>
-  </si>
-  <si>
-    <t>ציוד משרדי</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-003.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-07</t>
-  </si>
-  <si>
-    <t>חברת חשמל</t>
-  </si>
-  <si>
-    <t>חשבונות</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-004.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-09</t>
-  </si>
-  <si>
-    <t>GitHub Enterprise</t>
-  </si>
-  <si>
-    <t>תוכנה</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-005.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-11</t>
-  </si>
-  <si>
-    <t>משרד עורך דין</t>
-  </si>
-  <si>
-    <t>שירותים משפטיים</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-006.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-13</t>
-  </si>
-  <si>
-    <t>LinkedIn Premium</t>
-  </si>
-  <si>
-    <t>שיווק</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-007.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-15</t>
-  </si>
-  <si>
-    <t>בזק בינלאומי</t>
-  </si>
-  <si>
-    <t>תקשורת</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-008.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-17</t>
-  </si>
-  <si>
-    <t>Adobe Creative Cloud</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-009.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-19</t>
-  </si>
-  <si>
-    <t>משלוח ארוחות</t>
-  </si>
-  <si>
-    <t>מזומן</t>
-  </si>
-  <si>
-    <t>אירוח</t>
-  </si>
-  <si>
-    <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-010.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-21</t>
-  </si>
-  <si>
-    <t>AWS</t>
-  </si>
-  <si>
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-011.pdf</t>
   </si>
   <si>
-    <t>2025-12-23</t>
+    <t>2026-01-23</t>
   </si>
   <si>
     <t>חניון חודשי</t>
@@ -236,7 +251,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-012.pdf</t>
   </si>
   <si>
-    <t>2025-12-25</t>
+    <t>2026-01-25</t>
   </si>
   <si>
     <t>Zoom Pro</t>
@@ -245,7 +260,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-013.pdf</t>
   </si>
   <si>
-    <t>2025-12-27</t>
+    <t>2026-01-27</t>
   </si>
   <si>
     <t>ביטוח לאומי</t>
@@ -257,7 +272,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-014.pdf</t>
   </si>
   <si>
-    <t>2025-12-29</t>
+    <t>2026-01-29</t>
   </si>
   <si>
     <t>ניקיון משרדים</t>
@@ -677,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="1"/>
   </sheetViews>
@@ -744,32 +759,40 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B11">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -801,370 +824,370 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5">
         <v>4500</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5">
         <v>3200</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5">
         <v>850</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5">
         <v>650</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5">
         <v>1800</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5">
         <v>4200</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5">
         <v>350</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5">
         <v>450</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C10" s="5">
         <v>1000</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5">
         <v>950</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C12" s="5">
         <v>850</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C13" s="5">
         <v>700</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C14" s="5">
         <v>550</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C15" s="5">
         <v>3600</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C16" s="5">
         <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>